<commit_message>
#fix every day report
</commit_message>
<xml_diff>
--- a/storage/app/exel_templates/every_day_report.xlsx
+++ b/storage/app/exel_templates/every_day_report.xlsx
@@ -24,12 +24,6 @@
     <t>%day% %month% %year%</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Оператор</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>%product.date%</t>
   </si>
   <si>
-    <t>%product.index%</t>
-  </si>
-  <si>
     <t>%product.operator%</t>
   </si>
   <si>
@@ -139,6 +130,15 @@
   </si>
   <si>
     <t>%product.test%</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Статус</t>
+  </si>
+  <si>
+    <t>%product.status%</t>
   </si>
 </sst>
 </file>
@@ -271,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -282,6 +282,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -585,23 +586,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
     <col min="7" max="8" width="27.42578125" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
     <col min="11" max="11" width="27.85546875" customWidth="1"/>
     <col min="12" max="12" width="37.140625" customWidth="1"/>
-    <col min="13" max="13" width="28" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
     <col min="23" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -615,123 +623,123 @@
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="T6" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="N7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="P7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="Q7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="R7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="S7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="T7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="W7" t="s">
         <v>37</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="W7" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>